<commit_message>
fix the additional result function for revision
</commit_message>
<xml_diff>
--- a/documents/concepts/concepts.xlsx
+++ b/documents/concepts/concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apple\git\chandryou\TicagrelorVsClopidogrel\documents\concepts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apple\git\ohdsi-studies\TicagrelorVsClopidogrel\documents\concepts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B63C515-C72F-4BF4-B86A-2E6F3435D49C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A24E7B5-7249-4E01-8700-DA635C386FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{B68ED540-4C67-41CB-900F-2EA1B61F8C44}"/>
+    <workbookView xWindow="630" yWindow="10575" windowWidth="21600" windowHeight="11385" xr2:uid="{B68ED540-4C67-41CB-900F-2EA1B61F8C44}"/>
   </bookViews>
   <sheets>
     <sheet name="PCI" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1536,13 +1538,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA855CE4-BE17-46AA-A835-4630657CBE10}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4746,8 +4749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42375657-5F38-4314-BB53-931BC6CCD98C}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6778,11 +6781,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DD238F-D831-4B58-9A36-490ADBE5F1E0}">
   <dimension ref="A1:G215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>